<commit_message>
Space and Time Complexity Chart According to Contraints added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshi\OneDrive\Desktop\DSA450\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshad Joshi\Desktop\DSA_Cracker_Sheet_In_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="492">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1508,12 +1508,18 @@
   <si>
     <t xml:space="preserve"> First sort the array and then  </t>
   </si>
+  <si>
+    <t>Extended Merge Sort</t>
+  </si>
+  <si>
+    <t>To get maximum Profit we have to calculate minSoFar and maxProfitSoFar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1615,6 +1621,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1655,7 +1669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1697,6 +1711,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2016,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -2348,18 +2365,24 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="21">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="C21" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="21">
       <c r="A22" s="5" t="s">
@@ -2368,12 +2391,18 @@
       <c r="B22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="C22" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="21">
       <c r="A23" s="5" t="s">

</xml_diff>